<commit_message>
Criando classe do jogo
</commit_message>
<xml_diff>
--- a/archives/players.xlsx
+++ b/archives/players.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -575,6 +575,50 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>GABRIEL BONARETTI</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PEDRO</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implementando lógica do jogo e conectando classes
</commit_message>
<xml_diff>
--- a/archives/players.xlsx
+++ b/archives/players.xlsx
@@ -563,16 +563,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7">

</xml_diff>